<commit_message>
Lots of changes based on comments from reviewers
</commit_message>
<xml_diff>
--- a/Tables/Output/CXSPE_Supplemental_Tables.xlsx
+++ b/Tables/Output/CXSPE_Supplemental_Tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/j_sacks/Documents/GitHub/CX_SPE_Method/Tables/Output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F9A6AE7-25CA-D144-9031-11A737C73DF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BBA6143-68EB-5446-8935-F4A060DB61BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13360" yWindow="1460" windowWidth="15060" windowHeight="15740" activeTab="4" xr2:uid="{D8E72CCD-D09C-844F-BB4C-CE2C5BFA267B}"/>
+    <workbookView xWindow="13360" yWindow="1460" windowWidth="15060" windowHeight="15740" activeTab="6" xr2:uid="{D8E72CCD-D09C-844F-BB4C-CE2C5BFA267B}"/>
   </bookViews>
   <sheets>
     <sheet name="TableS1" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2719" uniqueCount="624">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3092" uniqueCount="669">
   <si>
     <t>Spike-Before</t>
   </si>
@@ -1913,6 +1913,141 @@
   </si>
   <si>
     <t>ND</t>
+  </si>
+  <si>
+    <t>Mean Concentration (nM)</t>
+  </si>
+  <si>
+    <t>Standard Deviation of Concentration (nM)</t>
+  </si>
+  <si>
+    <t>Mean Concentration C (nM C)</t>
+  </si>
+  <si>
+    <t>Standard Deviation of Concentration C (nM C)</t>
+  </si>
+  <si>
+    <t>Mean Concentration N (nM N)</t>
+  </si>
+  <si>
+    <t>Standard Deviation of Concentration N (nM N)</t>
+  </si>
+  <si>
+    <t>(3-Carboxypropyl)trimethylammonium (TMAB)</t>
+  </si>
+  <si>
+    <t>Aloha</t>
+  </si>
+  <si>
+    <t>4-Hydroxyisoleucine</t>
+  </si>
+  <si>
+    <t>6-Methyladenine</t>
+  </si>
+  <si>
+    <t>Asparagine</t>
+  </si>
+  <si>
+    <t>Aspartic acid</t>
+  </si>
+  <si>
+    <t>Dimethylsulfonioacetate (DMS-Ac)</t>
+  </si>
+  <si>
+    <t>DMSP</t>
+  </si>
+  <si>
+    <t>Glutamic acid</t>
+  </si>
+  <si>
+    <t>Glutamine</t>
+  </si>
+  <si>
+    <t>Histidine</t>
+  </si>
+  <si>
+    <t>Homoserine</t>
+  </si>
+  <si>
+    <t>Hydroxyectoine</t>
+  </si>
+  <si>
+    <t>Imidazoleacrylic Acid</t>
+  </si>
+  <si>
+    <t>(Iso)leucine</t>
+  </si>
+  <si>
+    <t>Lysine</t>
+  </si>
+  <si>
+    <t>Methionine Sulfoxide</t>
+  </si>
+  <si>
+    <t>N(e)-Acetyl-Lysine</t>
+  </si>
+  <si>
+    <t>Ornithine</t>
+  </si>
+  <si>
+    <t>Serine</t>
+  </si>
+  <si>
+    <t>Stachydrine hydrochloride</t>
+  </si>
+  <si>
+    <t>trans Hydroxyl proline</t>
+  </si>
+  <si>
+    <t>Trimethylammonium Propionate (TMAP)</t>
+  </si>
+  <si>
+    <t>Tyrosine</t>
+  </si>
+  <si>
+    <t>Alanine</t>
+  </si>
+  <si>
+    <t>Proline</t>
+  </si>
+  <si>
+    <t>Betaine</t>
+  </si>
+  <si>
+    <t>Phenylalanine</t>
+  </si>
+  <si>
+    <t>Applied LOD threshold (nM)</t>
+  </si>
+  <si>
+    <t>Aconitic Acid</t>
+  </si>
+  <si>
+    <t>Resorcylic Acid</t>
+  </si>
+  <si>
+    <t>Adenosyl Homocysteine</t>
+  </si>
+  <si>
+    <t>Domoic Acid</t>
+  </si>
+  <si>
+    <t>Kynurenine</t>
+  </si>
+  <si>
+    <t>Sulfurol</t>
+  </si>
+  <si>
+    <t>Vitamin B3</t>
+  </si>
+  <si>
+    <t>Vitamin B5</t>
+  </si>
+  <si>
+    <t>Vitamin B6</t>
+  </si>
+  <si>
+    <t>Vitamin B9</t>
   </si>
 </sst>
 </file>
@@ -14987,7 +15122,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6812D48-0DD4-2047-BF76-9276BB2150F5}">
   <dimension ref="A1:E142"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
@@ -17420,24 +17555,4430 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3A3D62B-683A-DE43-9952-34055B117537}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H120"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" t="s">
+        <v>616</v>
+      </c>
+      <c r="C1" t="s">
+        <v>624</v>
+      </c>
+      <c r="D1" t="s">
+        <v>625</v>
+      </c>
+      <c r="E1" t="s">
+        <v>626</v>
+      </c>
+      <c r="F1" t="s">
+        <v>627</v>
+      </c>
+      <c r="G1" t="s">
+        <v>628</v>
+      </c>
+      <c r="H1" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>630</v>
+      </c>
+      <c r="B2" t="s">
+        <v>631</v>
+      </c>
+      <c r="C2">
+        <v>4.7905447548750403E-2</v>
+      </c>
+      <c r="D2">
+        <v>3.8186541588685098E-3</v>
+      </c>
+      <c r="E2">
+        <v>0.33533813284125202</v>
+      </c>
+      <c r="F2">
+        <v>2.6730579112079499E-2</v>
+      </c>
+      <c r="G2">
+        <v>4.7905447548750403E-2</v>
+      </c>
+      <c r="H2">
+        <v>3.8186541588685098E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>630</v>
+      </c>
+      <c r="B3" t="s">
+        <v>620</v>
+      </c>
+      <c r="C3">
+        <v>3.3900792749077001E-2</v>
+      </c>
+      <c r="D3">
+        <v>5.5751604938848696E-3</v>
+      </c>
+      <c r="E3">
+        <v>0.237305549243539</v>
+      </c>
+      <c r="F3">
+        <v>3.9026123457194098E-2</v>
+      </c>
+      <c r="G3">
+        <v>3.3900792749077001E-2</v>
+      </c>
+      <c r="H3">
+        <v>5.5751604938848696E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>630</v>
+      </c>
+      <c r="B4" t="s">
+        <v>621</v>
+      </c>
+      <c r="C4">
+        <v>0.108878151424577</v>
+      </c>
+      <c r="D4">
+        <v>1.07742471355925E-2</v>
+      </c>
+      <c r="E4">
+        <v>0.76214705997204302</v>
+      </c>
+      <c r="F4">
+        <v>7.5419729949147502E-2</v>
+      </c>
+      <c r="G4">
+        <v>0.108878151424577</v>
+      </c>
+      <c r="H4">
+        <v>1.07742471355925E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>632</v>
+      </c>
+      <c r="B5" t="s">
+        <v>631</v>
+      </c>
+      <c r="C5">
+        <v>1.1397251389008101</v>
+      </c>
+      <c r="D5">
+        <v>0.23206322055108899</v>
+      </c>
+      <c r="E5">
+        <v>6.8383508334048999</v>
+      </c>
+      <c r="F5">
+        <v>1.39237932330653</v>
+      </c>
+      <c r="G5">
+        <v>1.1397251389008101</v>
+      </c>
+      <c r="H5">
+        <v>0.23206322055108899</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>632</v>
+      </c>
+      <c r="B6" t="s">
+        <v>622</v>
+      </c>
+      <c r="C6">
+        <v>2.2472004182706602</v>
+      </c>
+      <c r="D6">
+        <v>0.67707599909309601</v>
+      </c>
+      <c r="E6">
+        <v>13.483202509623901</v>
+      </c>
+      <c r="F6">
+        <v>4.0624559945585803</v>
+      </c>
+      <c r="G6">
+        <v>2.2472004182706602</v>
+      </c>
+      <c r="H6">
+        <v>0.67707599909309601</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>351</v>
+      </c>
+      <c r="B7" t="s">
+        <v>622</v>
+      </c>
+      <c r="C7">
+        <v>8.6613064357813102E-2</v>
+      </c>
+      <c r="D7">
+        <v>1.3894601270863401E-2</v>
+      </c>
+      <c r="E7">
+        <v>0.43306532178906498</v>
+      </c>
+      <c r="F7">
+        <v>6.9473006354317204E-2</v>
+      </c>
+      <c r="G7">
+        <v>0.259839193073439</v>
+      </c>
+      <c r="H7">
+        <v>4.1683803812590299E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>633</v>
+      </c>
+      <c r="B8" t="s">
+        <v>622</v>
+      </c>
+      <c r="C8">
+        <v>5.7243422724463998E-2</v>
+      </c>
+      <c r="D8">
+        <v>3.23672638493777E-2</v>
+      </c>
+      <c r="E8">
+        <v>0.34346053634678397</v>
+      </c>
+      <c r="F8">
+        <v>0.19420358309626601</v>
+      </c>
+      <c r="G8">
+        <v>0.28621711362232</v>
+      </c>
+      <c r="H8">
+        <v>0.16183631924688799</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>390</v>
+      </c>
+      <c r="B9" t="s">
+        <v>622</v>
+      </c>
+      <c r="C9">
+        <v>0.48847242679390401</v>
+      </c>
+      <c r="D9">
+        <v>0.18614761501825899</v>
+      </c>
+      <c r="E9">
+        <v>2.4423621339695201</v>
+      </c>
+      <c r="F9">
+        <v>0.93073807509129602</v>
+      </c>
+      <c r="G9">
+        <v>2.4423621339695201</v>
+      </c>
+      <c r="H9">
+        <v>0.93073807509129602</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>400</v>
+      </c>
+      <c r="B10" t="s">
+        <v>622</v>
+      </c>
+      <c r="C10">
+        <v>1.8801118516119899</v>
+      </c>
+      <c r="D10">
+        <v>0.52615213835192598</v>
+      </c>
+      <c r="E10">
+        <v>18.801118516119899</v>
+      </c>
+      <c r="F10">
+        <v>5.26152138351926</v>
+      </c>
+      <c r="G10">
+        <v>9.4005592580599497</v>
+      </c>
+      <c r="H10">
+        <v>2.63076069175963</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>634</v>
+      </c>
+      <c r="B11" t="s">
+        <v>631</v>
+      </c>
+      <c r="C11">
+        <v>2.1911365692202001</v>
+      </c>
+      <c r="D11">
+        <v>0.16476279109253</v>
+      </c>
+      <c r="E11">
+        <v>8.7645462768808002</v>
+      </c>
+      <c r="F11">
+        <v>0.65905116437012201</v>
+      </c>
+      <c r="G11">
+        <v>4.3822731384404001</v>
+      </c>
+      <c r="H11">
+        <v>0.32952558218506101</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>634</v>
+      </c>
+      <c r="B12" t="s">
+        <v>622</v>
+      </c>
+      <c r="C12">
+        <v>1.28617903416799</v>
+      </c>
+      <c r="D12">
+        <v>0.17845506580624801</v>
+      </c>
+      <c r="E12">
+        <v>5.1447161366719598</v>
+      </c>
+      <c r="F12">
+        <v>0.71382026322499403</v>
+      </c>
+      <c r="G12">
+        <v>2.5723580683359799</v>
+      </c>
+      <c r="H12">
+        <v>0.35691013161249702</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>635</v>
+      </c>
+      <c r="B13" t="s">
+        <v>631</v>
+      </c>
+      <c r="C13">
+        <v>6.7264770597718702</v>
+      </c>
+      <c r="D13">
+        <v>1.26636833484815</v>
+      </c>
+      <c r="E13">
+        <v>26.905908239087498</v>
+      </c>
+      <c r="F13">
+        <v>5.0654733393926001</v>
+      </c>
+      <c r="G13">
+        <v>6.7264770597718702</v>
+      </c>
+      <c r="H13">
+        <v>1.26636833484815</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>635</v>
+      </c>
+      <c r="B14" t="s">
+        <v>622</v>
+      </c>
+      <c r="C14">
+        <v>6.0789729310051097</v>
+      </c>
+      <c r="D14">
+        <v>2.0240984197187801</v>
+      </c>
+      <c r="E14">
+        <v>24.3158917240204</v>
+      </c>
+      <c r="F14">
+        <v>8.0963936788751507</v>
+      </c>
+      <c r="G14">
+        <v>6.0789729310051097</v>
+      </c>
+      <c r="H14">
+        <v>2.0240984197187801</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>635</v>
+      </c>
+      <c r="B15" t="s">
+        <v>621</v>
+      </c>
+      <c r="C15">
+        <v>7.0356145136348296</v>
+      </c>
+      <c r="D15">
+        <v>4.1812285641943499</v>
+      </c>
+      <c r="E15">
+        <v>28.142458054539301</v>
+      </c>
+      <c r="F15">
+        <v>16.724914256777399</v>
+      </c>
+      <c r="G15">
+        <v>7.0356145136348296</v>
+      </c>
+      <c r="H15">
+        <v>4.1812285641943499</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>314</v>
+      </c>
+      <c r="B16" t="s">
+        <v>631</v>
+      </c>
+      <c r="C16">
+        <v>2.1044495275758899</v>
+      </c>
+      <c r="D16">
+        <v>0.38076019659517801</v>
+      </c>
+      <c r="E16">
+        <v>6.3133485827276701</v>
+      </c>
+      <c r="F16">
+        <v>1.1422805897855299</v>
+      </c>
+      <c r="G16">
+        <v>2.1044495275758899</v>
+      </c>
+      <c r="H16">
+        <v>0.38076019659517801</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>314</v>
+      </c>
+      <c r="B17" t="s">
+        <v>620</v>
+      </c>
+      <c r="C17">
+        <v>1.7268133272184201</v>
+      </c>
+      <c r="D17">
+        <v>0.36806184271450099</v>
+      </c>
+      <c r="E17">
+        <v>5.1804399816552804</v>
+      </c>
+      <c r="F17">
+        <v>1.1041855281435</v>
+      </c>
+      <c r="G17">
+        <v>1.7268133272184201</v>
+      </c>
+      <c r="H17">
+        <v>0.36806184271450099</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>314</v>
+      </c>
+      <c r="B18" t="s">
+        <v>621</v>
+      </c>
+      <c r="C18">
+        <v>2.4841878556192301</v>
+      </c>
+      <c r="D18">
+        <v>0.62267929004390399</v>
+      </c>
+      <c r="E18">
+        <v>7.4525635668576999</v>
+      </c>
+      <c r="F18">
+        <v>1.86803787013171</v>
+      </c>
+      <c r="G18">
+        <v>2.4841878556192301</v>
+      </c>
+      <c r="H18">
+        <v>0.62267929004390399</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>316</v>
+      </c>
+      <c r="B19" t="s">
+        <v>631</v>
+      </c>
+      <c r="C19">
+        <v>6.11501329364472E-2</v>
+      </c>
+      <c r="D19">
+        <v>9.9776137107771695E-3</v>
+      </c>
+      <c r="E19">
+        <v>0.42805093055512999</v>
+      </c>
+      <c r="F19">
+        <v>6.9843295975440201E-2</v>
+      </c>
+      <c r="G19">
+        <v>6.11501329364472E-2</v>
+      </c>
+      <c r="H19">
+        <v>9.9776137107771695E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>316</v>
+      </c>
+      <c r="B20" t="s">
+        <v>622</v>
+      </c>
+      <c r="C20">
+        <v>1.7728765715729601E-2</v>
+      </c>
+      <c r="D20">
+        <v>5.5926444511736001E-3</v>
+      </c>
+      <c r="E20">
+        <v>0.12410136001010701</v>
+      </c>
+      <c r="F20">
+        <v>3.9148511158215202E-2</v>
+      </c>
+      <c r="G20">
+        <v>1.7728765715729601E-2</v>
+      </c>
+      <c r="H20">
+        <v>5.5926444511736001E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>316</v>
+      </c>
+      <c r="B21" t="s">
+        <v>620</v>
+      </c>
+      <c r="C21">
+        <v>1.9020957672192602E-2</v>
+      </c>
+      <c r="D21">
+        <v>6.8907584975203603E-3</v>
+      </c>
+      <c r="E21">
+        <v>0.13314670370534801</v>
+      </c>
+      <c r="F21">
+        <v>4.8235309482642499E-2</v>
+      </c>
+      <c r="G21">
+        <v>1.9020957672192602E-2</v>
+      </c>
+      <c r="H21">
+        <v>6.8907584975203603E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>316</v>
+      </c>
+      <c r="B22" t="s">
+        <v>621</v>
+      </c>
+      <c r="C22">
+        <v>1.5754482147189199E-2</v>
+      </c>
+      <c r="D22">
+        <v>3.5221425909293699E-3</v>
+      </c>
+      <c r="E22">
+        <v>0.11028137503032399</v>
+      </c>
+      <c r="F22">
+        <v>2.4654998136505599E-2</v>
+      </c>
+      <c r="G22">
+        <v>1.5754482147189199E-2</v>
+      </c>
+      <c r="H22">
+        <v>3.5221425909293699E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>438</v>
+      </c>
+      <c r="B23" t="s">
+        <v>631</v>
+      </c>
+      <c r="C23">
+        <v>0.89932725594499097</v>
+      </c>
+      <c r="D23">
+        <v>4.6548494139692503E-2</v>
+      </c>
+      <c r="E23">
+        <v>3.5973090237799599</v>
+      </c>
+      <c r="F23">
+        <v>0.18619397655877001</v>
+      </c>
+      <c r="G23">
+        <v>2.6979817678349698</v>
+      </c>
+      <c r="H23">
+        <v>0.13964548241907701</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>438</v>
+      </c>
+      <c r="B24" t="s">
+        <v>622</v>
+      </c>
+      <c r="C24">
+        <v>0.51699072593415796</v>
+      </c>
+      <c r="D24">
+        <v>0.187584962566715</v>
+      </c>
+      <c r="E24">
+        <v>2.0679629037366301</v>
+      </c>
+      <c r="F24">
+        <v>0.75033985026686301</v>
+      </c>
+      <c r="G24">
+        <v>1.5509721778024701</v>
+      </c>
+      <c r="H24">
+        <v>0.56275488770014703</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>438</v>
+      </c>
+      <c r="B25" t="s">
+        <v>620</v>
+      </c>
+      <c r="C25">
+        <v>0.410597280265733</v>
+      </c>
+      <c r="D25">
+        <v>9.9740926510723804E-2</v>
+      </c>
+      <c r="E25">
+        <v>1.64238912106293</v>
+      </c>
+      <c r="F25">
+        <v>0.39896370604289499</v>
+      </c>
+      <c r="G25">
+        <v>1.2317918407971999</v>
+      </c>
+      <c r="H25">
+        <v>0.29922277953217102</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>438</v>
+      </c>
+      <c r="B26" t="s">
+        <v>621</v>
+      </c>
+      <c r="C26">
+        <v>0.195561186556826</v>
+      </c>
+      <c r="D26">
+        <v>1.94383657245095E-2</v>
+      </c>
+      <c r="E26">
+        <v>0.782244746227305</v>
+      </c>
+      <c r="F26">
+        <v>7.7753462898038098E-2</v>
+      </c>
+      <c r="G26">
+        <v>0.58668355967047903</v>
+      </c>
+      <c r="H26">
+        <v>5.8315097173528598E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>402</v>
+      </c>
+      <c r="B27" t="s">
+        <v>622</v>
+      </c>
+      <c r="C27">
+        <v>0.54373586078843195</v>
+      </c>
+      <c r="D27">
+        <v>0.25393886002778998</v>
+      </c>
+      <c r="E27">
+        <v>4.89362274709588</v>
+      </c>
+      <c r="F27">
+        <v>2.2854497402501099</v>
+      </c>
+      <c r="G27">
+        <v>1.6312075823652901</v>
+      </c>
+      <c r="H27">
+        <v>0.76181658008337005</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>402</v>
+      </c>
+      <c r="B28" t="s">
+        <v>621</v>
+      </c>
+      <c r="C28">
+        <v>0.14707402105348999</v>
+      </c>
+      <c r="D28">
+        <v>1.69998707573366E-2</v>
+      </c>
+      <c r="E28">
+        <v>1.3236661894814099</v>
+      </c>
+      <c r="F28">
+        <v>0.15299883681602999</v>
+      </c>
+      <c r="G28">
+        <v>0.44122206316047002</v>
+      </c>
+      <c r="H28">
+        <v>5.0999612272009998E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>636</v>
+      </c>
+      <c r="B29" t="s">
+        <v>631</v>
+      </c>
+      <c r="C29">
+        <v>0.46393100499671502</v>
+      </c>
+      <c r="D29">
+        <v>2.0903992043633999E-2</v>
+      </c>
+      <c r="E29">
+        <v>1.8557240199868601</v>
+      </c>
+      <c r="F29">
+        <v>8.3615968174536301E-2</v>
+      </c>
+      <c r="G29" t="s">
+        <v>322</v>
+      </c>
+      <c r="H29" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>636</v>
+      </c>
+      <c r="B30" t="s">
+        <v>620</v>
+      </c>
+      <c r="C30">
+        <v>0.96473619858665705</v>
+      </c>
+      <c r="D30">
+        <v>0.218681890953142</v>
+      </c>
+      <c r="E30">
+        <v>3.8589447943466202</v>
+      </c>
+      <c r="F30">
+        <v>0.874727563812569</v>
+      </c>
+      <c r="G30" t="s">
+        <v>322</v>
+      </c>
+      <c r="H30" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>636</v>
+      </c>
+      <c r="B31" t="s">
+        <v>621</v>
+      </c>
+      <c r="C31">
+        <v>0.49629152816149302</v>
+      </c>
+      <c r="D31">
+        <v>4.3028145026474902E-2</v>
+      </c>
+      <c r="E31">
+        <v>1.9851661126459701</v>
+      </c>
+      <c r="F31">
+        <v>0.172112580105899</v>
+      </c>
+      <c r="G31" t="s">
+        <v>322</v>
+      </c>
+      <c r="H31" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>637</v>
+      </c>
+      <c r="B32" t="s">
+        <v>631</v>
+      </c>
+      <c r="C32">
+        <v>3.43083186661711</v>
+      </c>
+      <c r="D32">
+        <v>0.19681201908199</v>
+      </c>
+      <c r="E32">
+        <v>17.154159333085499</v>
+      </c>
+      <c r="F32">
+        <v>0.98406009540994999</v>
+      </c>
+      <c r="G32" t="s">
+        <v>322</v>
+      </c>
+      <c r="H32" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>637</v>
+      </c>
+      <c r="B33" t="s">
+        <v>622</v>
+      </c>
+      <c r="C33">
+        <v>1.31136498162357E-2</v>
+      </c>
+      <c r="D33">
+        <v>4.0780746152690502E-3</v>
+      </c>
+      <c r="E33">
+        <v>6.5568249081178503E-2</v>
+      </c>
+      <c r="F33">
+        <v>2.0390373076345201E-2</v>
+      </c>
+      <c r="G33" t="s">
+        <v>322</v>
+      </c>
+      <c r="H33" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>637</v>
+      </c>
+      <c r="B34" t="s">
+        <v>620</v>
+      </c>
+      <c r="C34">
+        <v>6.6951519237724701</v>
+      </c>
+      <c r="D34">
+        <v>1.45016385946829</v>
+      </c>
+      <c r="E34">
+        <v>33.475759618862298</v>
+      </c>
+      <c r="F34">
+        <v>7.25081929734145</v>
+      </c>
+      <c r="G34" t="s">
+        <v>322</v>
+      </c>
+      <c r="H34" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>637</v>
+      </c>
+      <c r="B35" t="s">
+        <v>621</v>
+      </c>
+      <c r="C35">
+        <v>2.25886574689165</v>
+      </c>
+      <c r="D35">
+        <v>0.25798206234176801</v>
+      </c>
+      <c r="E35">
+        <v>11.294328734458199</v>
+      </c>
+      <c r="F35">
+        <v>1.28991031170884</v>
+      </c>
+      <c r="G35" t="s">
+        <v>322</v>
+      </c>
+      <c r="H35" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>444</v>
+      </c>
+      <c r="B36" t="s">
+        <v>631</v>
+      </c>
+      <c r="C36">
+        <v>5.4408310755174397E-2</v>
+      </c>
+      <c r="D36">
+        <v>4.12823918474939E-3</v>
+      </c>
+      <c r="E36">
+        <v>0.32644986453104602</v>
+      </c>
+      <c r="F36">
+        <v>2.4769435108496302E-2</v>
+      </c>
+      <c r="G36">
+        <v>0.108816621510348</v>
+      </c>
+      <c r="H36">
+        <v>8.2564783694987903E-3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>444</v>
+      </c>
+      <c r="B37" t="s">
+        <v>620</v>
+      </c>
+      <c r="C37">
+        <v>4.5913136932276097E-2</v>
+      </c>
+      <c r="D37">
+        <v>5.0281206855579798E-3</v>
+      </c>
+      <c r="E37">
+        <v>0.275478821593656</v>
+      </c>
+      <c r="F37">
+        <v>3.0168724113347901E-2</v>
+      </c>
+      <c r="G37">
+        <v>9.1826273864552305E-2</v>
+      </c>
+      <c r="H37">
+        <v>1.0056241371115901E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>638</v>
+      </c>
+      <c r="B38" t="s">
+        <v>631</v>
+      </c>
+      <c r="C38">
+        <v>11.408896124196101</v>
+      </c>
+      <c r="D38">
+        <v>1.7374641596409199</v>
+      </c>
+      <c r="E38">
+        <v>57.044480620980799</v>
+      </c>
+      <c r="F38">
+        <v>8.6873207982046292</v>
+      </c>
+      <c r="G38">
+        <v>11.408896124196101</v>
+      </c>
+      <c r="H38">
+        <v>1.7374641596409199</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>638</v>
+      </c>
+      <c r="B39" t="s">
+        <v>622</v>
+      </c>
+      <c r="C39">
+        <v>5.6779624653213903</v>
+      </c>
+      <c r="D39">
+        <v>0.427917454783173</v>
+      </c>
+      <c r="E39">
+        <v>28.389812326606901</v>
+      </c>
+      <c r="F39">
+        <v>2.1395872739158599</v>
+      </c>
+      <c r="G39">
+        <v>5.6779624653213903</v>
+      </c>
+      <c r="H39">
+        <v>0.427917454783173</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>638</v>
+      </c>
+      <c r="B40" t="s">
+        <v>620</v>
+      </c>
+      <c r="C40">
+        <v>3.19501751775742</v>
+      </c>
+      <c r="D40">
+        <v>0.84916747920225899</v>
+      </c>
+      <c r="E40">
+        <v>15.975087588787099</v>
+      </c>
+      <c r="F40">
+        <v>4.2458373960112903</v>
+      </c>
+      <c r="G40">
+        <v>3.19501751775742</v>
+      </c>
+      <c r="H40">
+        <v>0.84916747920225899</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>638</v>
+      </c>
+      <c r="B41" t="s">
+        <v>621</v>
+      </c>
+      <c r="C41">
+        <v>4.76816888364728</v>
+      </c>
+      <c r="D41">
+        <v>0.48620310333149702</v>
+      </c>
+      <c r="E41">
+        <v>23.840844418236401</v>
+      </c>
+      <c r="F41">
+        <v>2.4310155166574798</v>
+      </c>
+      <c r="G41">
+        <v>4.76816888364728</v>
+      </c>
+      <c r="H41">
+        <v>0.48620310333149702</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>639</v>
+      </c>
+      <c r="B42" t="s">
+        <v>631</v>
+      </c>
+      <c r="C42">
+        <v>1.0051424335777901</v>
+      </c>
+      <c r="D42">
+        <v>9.5892125209311396E-2</v>
+      </c>
+      <c r="E42">
+        <v>5.02571216788896</v>
+      </c>
+      <c r="F42">
+        <v>0.47946062604655698</v>
+      </c>
+      <c r="G42">
+        <v>2.0102848671555802</v>
+      </c>
+      <c r="H42">
+        <v>0.19178425041862199</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>639</v>
+      </c>
+      <c r="B43" t="s">
+        <v>622</v>
+      </c>
+      <c r="C43">
+        <v>0.34156501882253298</v>
+      </c>
+      <c r="D43">
+        <v>9.9238219500793104E-2</v>
+      </c>
+      <c r="E43">
+        <v>1.70782509411266</v>
+      </c>
+      <c r="F43">
+        <v>0.49619109750396501</v>
+      </c>
+      <c r="G43">
+        <v>0.68313003764506697</v>
+      </c>
+      <c r="H43">
+        <v>0.19847643900158601</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>639</v>
+      </c>
+      <c r="B44" t="s">
+        <v>620</v>
+      </c>
+      <c r="C44">
+        <v>0.14950592610828001</v>
+      </c>
+      <c r="D44">
+        <v>6.5620546020115703E-2</v>
+      </c>
+      <c r="E44">
+        <v>0.74752963054139998</v>
+      </c>
+      <c r="F44">
+        <v>0.328102730100578</v>
+      </c>
+      <c r="G44">
+        <v>0.29901185221656001</v>
+      </c>
+      <c r="H44">
+        <v>0.13124109204023099</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>639</v>
+      </c>
+      <c r="B45" t="s">
+        <v>621</v>
+      </c>
+      <c r="C45">
+        <v>0.62007671574940404</v>
+      </c>
+      <c r="D45">
+        <v>2.6306126352886199E-2</v>
+      </c>
+      <c r="E45">
+        <v>3.10038357874702</v>
+      </c>
+      <c r="F45">
+        <v>0.131530631764431</v>
+      </c>
+      <c r="G45">
+        <v>1.2401534314988001</v>
+      </c>
+      <c r="H45">
+        <v>5.2612252705772501E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>379</v>
+      </c>
+      <c r="B46" t="s">
+        <v>631</v>
+      </c>
+      <c r="C46">
+        <v>5.4738563747535197E-2</v>
+      </c>
+      <c r="D46">
+        <v>1.6498539961250901E-2</v>
+      </c>
+      <c r="E46">
+        <v>0.76633989246549294</v>
+      </c>
+      <c r="F46">
+        <v>0.230979559457513</v>
+      </c>
+      <c r="G46">
+        <v>0.10947712749507001</v>
+      </c>
+      <c r="H46">
+        <v>3.29970799225019E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>379</v>
+      </c>
+      <c r="B47" t="s">
+        <v>621</v>
+      </c>
+      <c r="C47">
+        <v>5.4691987185650298E-2</v>
+      </c>
+      <c r="D47">
+        <v>1.23716532030706E-2</v>
+      </c>
+      <c r="E47">
+        <v>0.76568782059910501</v>
+      </c>
+      <c r="F47">
+        <v>0.17320314484298899</v>
+      </c>
+      <c r="G47">
+        <v>0.1093839743713</v>
+      </c>
+      <c r="H47">
+        <v>2.4743306406141301E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>298</v>
+      </c>
+      <c r="B48" t="s">
+        <v>621</v>
+      </c>
+      <c r="C48">
+        <v>1.3867722864397101</v>
+      </c>
+      <c r="D48">
+        <v>8.7247935832097195E-2</v>
+      </c>
+      <c r="E48">
+        <v>11.094178291517601</v>
+      </c>
+      <c r="F48">
+        <v>0.69798348665677801</v>
+      </c>
+      <c r="G48">
+        <v>1.3867722864397101</v>
+      </c>
+      <c r="H48">
+        <v>8.7247935832097195E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>323</v>
+      </c>
+      <c r="B49" t="s">
+        <v>631</v>
+      </c>
+      <c r="C49">
+        <v>0.60698229132119497</v>
+      </c>
+      <c r="D49">
+        <v>5.61376801468014E-2</v>
+      </c>
+      <c r="E49">
+        <v>4.2488760392483602</v>
+      </c>
+      <c r="F49">
+        <v>0.39296376102760899</v>
+      </c>
+      <c r="G49" t="s">
+        <v>322</v>
+      </c>
+      <c r="H49" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>323</v>
+      </c>
+      <c r="B50" t="s">
+        <v>622</v>
+      </c>
+      <c r="C50">
+        <v>0.85749377941112104</v>
+      </c>
+      <c r="D50">
+        <v>0.33601718434847699</v>
+      </c>
+      <c r="E50">
+        <v>6.0024564558778497</v>
+      </c>
+      <c r="F50">
+        <v>2.3521202904393399</v>
+      </c>
+      <c r="G50" t="s">
+        <v>322</v>
+      </c>
+      <c r="H50" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>323</v>
+      </c>
+      <c r="B51" t="s">
+        <v>621</v>
+      </c>
+      <c r="C51">
+        <v>1.4697477553884499</v>
+      </c>
+      <c r="D51">
+        <v>0.20615026621299301</v>
+      </c>
+      <c r="E51">
+        <v>10.288234287719099</v>
+      </c>
+      <c r="F51">
+        <v>1.4430518634909499</v>
+      </c>
+      <c r="G51" t="s">
+        <v>322</v>
+      </c>
+      <c r="H51" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>394</v>
+      </c>
+      <c r="B52" t="s">
+        <v>631</v>
+      </c>
+      <c r="C52">
+        <v>0.78421598395490899</v>
+      </c>
+      <c r="D52">
+        <v>6.6697637635072901E-2</v>
+      </c>
+      <c r="E52">
+        <v>3.9210799197745398</v>
+      </c>
+      <c r="F52">
+        <v>0.33348818817536502</v>
+      </c>
+      <c r="G52">
+        <v>3.9210799197745398</v>
+      </c>
+      <c r="H52">
+        <v>0.33348818817536502</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>394</v>
+      </c>
+      <c r="B53" t="s">
+        <v>622</v>
+      </c>
+      <c r="C53">
+        <v>1.54307841812931</v>
+      </c>
+      <c r="D53">
+        <v>0.53086499722632896</v>
+      </c>
+      <c r="E53">
+        <v>7.7153920906465903</v>
+      </c>
+      <c r="F53">
+        <v>2.6543249861316398</v>
+      </c>
+      <c r="G53">
+        <v>7.7153920906465903</v>
+      </c>
+      <c r="H53">
+        <v>2.6543249861316398</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>394</v>
+      </c>
+      <c r="B54" t="s">
+        <v>621</v>
+      </c>
+      <c r="C54">
+        <v>1.02480210680191</v>
+      </c>
+      <c r="D54">
+        <v>5.5678782201437502E-2</v>
+      </c>
+      <c r="E54">
+        <v>5.1240105340095896</v>
+      </c>
+      <c r="F54">
+        <v>0.27839391100718702</v>
+      </c>
+      <c r="G54">
+        <v>5.1240105340095896</v>
+      </c>
+      <c r="H54">
+        <v>0.27839391100718702</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>640</v>
+      </c>
+      <c r="B55" t="s">
+        <v>631</v>
+      </c>
+      <c r="C55">
+        <v>1.2052798219893299</v>
+      </c>
+      <c r="D55">
+        <v>0.294374634707814</v>
+      </c>
+      <c r="E55">
+        <v>7.2316789319360097</v>
+      </c>
+      <c r="F55">
+        <v>1.76624780824688</v>
+      </c>
+      <c r="G55">
+        <v>3.615839465968</v>
+      </c>
+      <c r="H55">
+        <v>0.88312390412344399</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>640</v>
+      </c>
+      <c r="B56" t="s">
+        <v>622</v>
+      </c>
+      <c r="C56">
+        <v>2.09355692749065</v>
+      </c>
+      <c r="D56">
+        <v>0.116929041016227</v>
+      </c>
+      <c r="E56">
+        <v>12.5613415649439</v>
+      </c>
+      <c r="F56">
+        <v>0.70157424609736396</v>
+      </c>
+      <c r="G56">
+        <v>6.2806707824719599</v>
+      </c>
+      <c r="H56">
+        <v>0.35078712304868098</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>446</v>
+      </c>
+      <c r="B57" t="s">
+        <v>631</v>
+      </c>
+      <c r="C57">
+        <v>67.640912803089606</v>
+      </c>
+      <c r="D57">
+        <v>3.7625442531820399</v>
+      </c>
+      <c r="E57">
+        <v>473.48638962162698</v>
+      </c>
+      <c r="F57">
+        <v>26.337809772274301</v>
+      </c>
+      <c r="G57">
+        <v>67.640912803089606</v>
+      </c>
+      <c r="H57">
+        <v>3.7625442531820399</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>446</v>
+      </c>
+      <c r="B58" t="s">
+        <v>622</v>
+      </c>
+      <c r="C58">
+        <v>3.97542110858724</v>
+      </c>
+      <c r="D58">
+        <v>1.14208768495985</v>
+      </c>
+      <c r="E58">
+        <v>27.8279477601107</v>
+      </c>
+      <c r="F58">
+        <v>7.9946137947189602</v>
+      </c>
+      <c r="G58">
+        <v>3.97542110858724</v>
+      </c>
+      <c r="H58">
+        <v>1.14208768495985</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>446</v>
+      </c>
+      <c r="B59" t="s">
+        <v>620</v>
+      </c>
+      <c r="C59">
+        <v>20.842149070438101</v>
+      </c>
+      <c r="D59">
+        <v>4.6644384101801499</v>
+      </c>
+      <c r="E59">
+        <v>145.89504349306699</v>
+      </c>
+      <c r="F59">
+        <v>32.651068871261003</v>
+      </c>
+      <c r="G59">
+        <v>20.842149070438101</v>
+      </c>
+      <c r="H59">
+        <v>4.6644384101801499</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>446</v>
+      </c>
+      <c r="B60" t="s">
+        <v>621</v>
+      </c>
+      <c r="C60">
+        <v>40.409783137836101</v>
+      </c>
+      <c r="D60">
+        <v>5.4568687438241001</v>
+      </c>
+      <c r="E60">
+        <v>282.86848196485198</v>
+      </c>
+      <c r="F60">
+        <v>38.198081206768698</v>
+      </c>
+      <c r="G60">
+        <v>40.409783137836101</v>
+      </c>
+      <c r="H60">
+        <v>5.4568687438241001</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>641</v>
+      </c>
+      <c r="B61" t="s">
+        <v>621</v>
+      </c>
+      <c r="C61">
+        <v>0.47891855203238998</v>
+      </c>
+      <c r="D61">
+        <v>0.17072760872968701</v>
+      </c>
+      <c r="E61">
+        <v>1.9156742081295599</v>
+      </c>
+      <c r="F61">
+        <v>0.68291043491875003</v>
+      </c>
+      <c r="G61">
+        <v>0.47891855203238998</v>
+      </c>
+      <c r="H61">
+        <v>0.17072760872968701</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>642</v>
+      </c>
+      <c r="B62" t="s">
+        <v>621</v>
+      </c>
+      <c r="C62">
+        <v>5.18761097941167E-2</v>
+      </c>
+      <c r="D62">
+        <v>9.8624781766979992E-3</v>
+      </c>
+      <c r="E62">
+        <v>0.31125665876469999</v>
+      </c>
+      <c r="F62">
+        <v>5.9174869060187998E-2</v>
+      </c>
+      <c r="G62">
+        <v>0.103752219588233</v>
+      </c>
+      <c r="H62">
+        <v>1.9724956353395998E-2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>359</v>
+      </c>
+      <c r="B63" t="s">
+        <v>631</v>
+      </c>
+      <c r="C63">
+        <v>0.68656545517350698</v>
+      </c>
+      <c r="D63">
+        <v>0.116510732417756</v>
+      </c>
+      <c r="E63">
+        <v>3.4328272758675298</v>
+      </c>
+      <c r="F63">
+        <v>0.58255366208878201</v>
+      </c>
+      <c r="G63">
+        <v>2.7462618206940301</v>
+      </c>
+      <c r="H63">
+        <v>0.46604292967102601</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>359</v>
+      </c>
+      <c r="B64" t="s">
+        <v>622</v>
+      </c>
+      <c r="C64">
+        <v>1.3291731745715001</v>
+      </c>
+      <c r="D64">
+        <v>0.53787844796505102</v>
+      </c>
+      <c r="E64">
+        <v>6.6458658728575299</v>
+      </c>
+      <c r="F64">
+        <v>2.6893922398252501</v>
+      </c>
+      <c r="G64">
+        <v>5.3166926982860296</v>
+      </c>
+      <c r="H64">
+        <v>2.1515137918602001</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>643</v>
+      </c>
+      <c r="B65" t="s">
+        <v>631</v>
+      </c>
+      <c r="C65">
+        <v>1.5864593540654</v>
+      </c>
+      <c r="D65">
+        <v>0.49341457442165099</v>
+      </c>
+      <c r="E65">
+        <v>9.5187561243924499</v>
+      </c>
+      <c r="F65">
+        <v>2.9604874465298998</v>
+      </c>
+      <c r="G65">
+        <v>3.1729187081308101</v>
+      </c>
+      <c r="H65">
+        <v>0.98682914884330197</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>643</v>
+      </c>
+      <c r="B66" t="s">
+        <v>622</v>
+      </c>
+      <c r="C66">
+        <v>1.49270653316247</v>
+      </c>
+      <c r="D66">
+        <v>0.38129156965981797</v>
+      </c>
+      <c r="E66">
+        <v>8.9562391989748207</v>
+      </c>
+      <c r="F66">
+        <v>2.28774941795891</v>
+      </c>
+      <c r="G66">
+        <v>2.9854130663249401</v>
+      </c>
+      <c r="H66">
+        <v>0.76258313931963695</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>644</v>
+      </c>
+      <c r="B67" t="s">
+        <v>631</v>
+      </c>
+      <c r="C67">
+        <v>4.4283993488205002</v>
+      </c>
+      <c r="D67">
+        <v>0.19215130808824801</v>
+      </c>
+      <c r="E67">
+        <v>26.570396092923001</v>
+      </c>
+      <c r="F67">
+        <v>1.1529078485294799</v>
+      </c>
+      <c r="G67">
+        <v>4.4283993488205002</v>
+      </c>
+      <c r="H67">
+        <v>0.19215130808824801</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>644</v>
+      </c>
+      <c r="B68" t="s">
+        <v>622</v>
+      </c>
+      <c r="C68">
+        <v>1.3892635094363599</v>
+      </c>
+      <c r="D68">
+        <v>0.39081819803052897</v>
+      </c>
+      <c r="E68">
+        <v>8.3355810566181692</v>
+      </c>
+      <c r="F68">
+        <v>2.3449091881831698</v>
+      </c>
+      <c r="G68">
+        <v>1.3892635094363599</v>
+      </c>
+      <c r="H68">
+        <v>0.39081819803052897</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>644</v>
+      </c>
+      <c r="B69" t="s">
+        <v>620</v>
+      </c>
+      <c r="C69">
+        <v>0.53160865515893496</v>
+      </c>
+      <c r="D69">
+        <v>6.5957764227877094E-2</v>
+      </c>
+      <c r="E69">
+        <v>3.1896519309536102</v>
+      </c>
+      <c r="F69">
+        <v>0.39574658536726198</v>
+      </c>
+      <c r="G69">
+        <v>0.53160865515893496</v>
+      </c>
+      <c r="H69">
+        <v>6.5957764227877094E-2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>644</v>
+      </c>
+      <c r="B70" t="s">
+        <v>621</v>
+      </c>
+      <c r="C70">
+        <v>1.413867316433</v>
+      </c>
+      <c r="D70">
+        <v>2.7939701798335399E-2</v>
+      </c>
+      <c r="E70">
+        <v>8.48320389859804</v>
+      </c>
+      <c r="F70">
+        <v>0.16763821079001201</v>
+      </c>
+      <c r="G70">
+        <v>1.413867316433</v>
+      </c>
+      <c r="H70">
+        <v>2.7939701798335399E-2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>645</v>
+      </c>
+      <c r="B71" t="s">
+        <v>631</v>
+      </c>
+      <c r="C71">
+        <v>2.59260922981617</v>
+      </c>
+      <c r="D71">
+        <v>0.29622792980395701</v>
+      </c>
+      <c r="E71">
+        <v>15.555655378897001</v>
+      </c>
+      <c r="F71">
+        <v>1.77736757882374</v>
+      </c>
+      <c r="G71">
+        <v>5.1852184596323401</v>
+      </c>
+      <c r="H71">
+        <v>0.59245585960791503</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>334</v>
+      </c>
+      <c r="B72" t="s">
+        <v>631</v>
+      </c>
+      <c r="C72">
+        <v>0.90000922333664102</v>
+      </c>
+      <c r="D72">
+        <v>0.15708153547161199</v>
+      </c>
+      <c r="E72">
+        <v>2.7000276700099199</v>
+      </c>
+      <c r="F72">
+        <v>0.47124460641483601</v>
+      </c>
+      <c r="G72">
+        <v>5.4000553400198399</v>
+      </c>
+      <c r="H72">
+        <v>0.94248921282967302</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>334</v>
+      </c>
+      <c r="B73" t="s">
+        <v>622</v>
+      </c>
+      <c r="C73">
+        <v>0.49947118434037002</v>
+      </c>
+      <c r="D73">
+        <v>4.9425181069304797E-2</v>
+      </c>
+      <c r="E73">
+        <v>1.49841355302111</v>
+      </c>
+      <c r="F73">
+        <v>0.148275543207914</v>
+      </c>
+      <c r="G73">
+        <v>2.99682710604222</v>
+      </c>
+      <c r="H73">
+        <v>0.296551086415829</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>646</v>
+      </c>
+      <c r="B74" t="s">
+        <v>631</v>
+      </c>
+      <c r="C74">
+        <v>1.3800553841523999</v>
+      </c>
+      <c r="D74">
+        <v>0.214110184439569</v>
+      </c>
+      <c r="E74">
+        <v>6.9002769207620203</v>
+      </c>
+      <c r="F74">
+        <v>1.07055092219784</v>
+      </c>
+      <c r="G74">
+        <v>1.3800553841523999</v>
+      </c>
+      <c r="H74">
+        <v>0.214110184439569</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>646</v>
+      </c>
+      <c r="B75" t="s">
+        <v>622</v>
+      </c>
+      <c r="C75">
+        <v>0.30329041934261702</v>
+      </c>
+      <c r="D75">
+        <v>2.4726834318032302E-2</v>
+      </c>
+      <c r="E75">
+        <v>1.5164520967130799</v>
+      </c>
+      <c r="F75">
+        <v>0.123634171590161</v>
+      </c>
+      <c r="G75">
+        <v>0.30329041934261702</v>
+      </c>
+      <c r="H75">
+        <v>2.4726834318032302E-2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>646</v>
+      </c>
+      <c r="B76" t="s">
+        <v>621</v>
+      </c>
+      <c r="C76">
+        <v>0.56110133165512199</v>
+      </c>
+      <c r="D76">
+        <v>0.171489540268632</v>
+      </c>
+      <c r="E76">
+        <v>2.8055066582756099</v>
+      </c>
+      <c r="F76">
+        <v>0.85744770134315995</v>
+      </c>
+      <c r="G76">
+        <v>0.56110133165512199</v>
+      </c>
+      <c r="H76">
+        <v>0.171489540268632</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>647</v>
+      </c>
+      <c r="B77" t="s">
+        <v>631</v>
+      </c>
+      <c r="C77">
+        <v>8.5164435074142897E-2</v>
+      </c>
+      <c r="D77">
+        <v>1.8394873186443301E-2</v>
+      </c>
+      <c r="E77">
+        <v>0.68131548059314295</v>
+      </c>
+      <c r="F77">
+        <v>0.14715898549154599</v>
+      </c>
+      <c r="G77">
+        <v>0.17032887014828499</v>
+      </c>
+      <c r="H77">
+        <v>3.6789746372886602E-2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>647</v>
+      </c>
+      <c r="B78" t="s">
+        <v>622</v>
+      </c>
+      <c r="C78">
+        <v>4.90978844387897E-2</v>
+      </c>
+      <c r="D78">
+        <v>2.2505040618637201E-2</v>
+      </c>
+      <c r="E78">
+        <v>0.39278307551031799</v>
+      </c>
+      <c r="F78">
+        <v>0.180040324949098</v>
+      </c>
+      <c r="G78">
+        <v>9.8195768877579498E-2</v>
+      </c>
+      <c r="H78">
+        <v>4.5010081237274499E-2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>647</v>
+      </c>
+      <c r="B79" t="s">
+        <v>621</v>
+      </c>
+      <c r="C79">
+        <v>2.7499929814487501E-2</v>
+      </c>
+      <c r="D79">
+        <v>9.3864810182827507E-3</v>
+      </c>
+      <c r="E79">
+        <v>0.21999943851590001</v>
+      </c>
+      <c r="F79">
+        <v>7.5091848146261894E-2</v>
+      </c>
+      <c r="G79">
+        <v>5.4999859628975099E-2</v>
+      </c>
+      <c r="H79">
+        <v>1.8772962036565401E-2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>648</v>
+      </c>
+      <c r="B80" t="s">
+        <v>631</v>
+      </c>
+      <c r="C80">
+        <v>8.2705075554843095</v>
+      </c>
+      <c r="D80">
+        <v>0.515050986122357</v>
+      </c>
+      <c r="E80">
+        <v>41.352537777421503</v>
+      </c>
+      <c r="F80">
+        <v>2.5752549306117798</v>
+      </c>
+      <c r="G80">
+        <v>16.541015110968601</v>
+      </c>
+      <c r="H80">
+        <v>1.03010197224471</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>218</v>
+      </c>
+      <c r="B81" t="s">
+        <v>631</v>
+      </c>
+      <c r="C81">
+        <v>0.91704063468789498</v>
+      </c>
+      <c r="D81">
+        <v>0.29864158653409201</v>
+      </c>
+      <c r="E81">
+        <v>2.7511219040636798</v>
+      </c>
+      <c r="F81">
+        <v>0.89592475960227702</v>
+      </c>
+      <c r="G81">
+        <v>0.91704063468789498</v>
+      </c>
+      <c r="H81">
+        <v>0.29864158653409201</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>218</v>
+      </c>
+      <c r="B82" t="s">
+        <v>620</v>
+      </c>
+      <c r="C82">
+        <v>1.1631301511690499</v>
+      </c>
+      <c r="D82">
+        <v>0.375165676059522</v>
+      </c>
+      <c r="E82">
+        <v>3.48939045350716</v>
+      </c>
+      <c r="F82">
+        <v>1.1254970281785599</v>
+      </c>
+      <c r="G82">
+        <v>1.1631301511690499</v>
+      </c>
+      <c r="H82">
+        <v>0.375165676059522</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>649</v>
+      </c>
+      <c r="B83" t="s">
+        <v>631</v>
+      </c>
+      <c r="C83">
+        <v>13.5153494896756</v>
+      </c>
+      <c r="D83">
+        <v>5.0306486316400401</v>
+      </c>
+      <c r="E83">
+        <v>40.5460484690268</v>
+      </c>
+      <c r="F83">
+        <v>15.0919458949201</v>
+      </c>
+      <c r="G83">
+        <v>13.5153494896756</v>
+      </c>
+      <c r="H83">
+        <v>5.0306486316400401</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>649</v>
+      </c>
+      <c r="B84" t="s">
+        <v>622</v>
+      </c>
+      <c r="C84">
+        <v>16.552275387312999</v>
+      </c>
+      <c r="D84">
+        <v>3.7288484854027701</v>
+      </c>
+      <c r="E84">
+        <v>49.656826161939101</v>
+      </c>
+      <c r="F84">
+        <v>11.1865454562083</v>
+      </c>
+      <c r="G84">
+        <v>16.552275387312999</v>
+      </c>
+      <c r="H84">
+        <v>3.7288484854027701</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>650</v>
+      </c>
+      <c r="B85" t="s">
+        <v>631</v>
+      </c>
+      <c r="C85">
+        <v>0.14263965156810299</v>
+      </c>
+      <c r="D85">
+        <v>8.1056786198146994E-3</v>
+      </c>
+      <c r="E85">
+        <v>0.99847756097672502</v>
+      </c>
+      <c r="F85">
+        <v>5.67397503387028E-2</v>
+      </c>
+      <c r="G85">
+        <v>0.14263965156810299</v>
+      </c>
+      <c r="H85">
+        <v>8.1056786198146994E-3</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>650</v>
+      </c>
+      <c r="B86" t="s">
+        <v>621</v>
+      </c>
+      <c r="C86">
+        <v>4.99428592696275E-2</v>
+      </c>
+      <c r="D86">
+        <v>6.5068386110087298E-3</v>
+      </c>
+      <c r="E86">
+        <v>0.34960001488739201</v>
+      </c>
+      <c r="F86">
+        <v>4.55478702770611E-2</v>
+      </c>
+      <c r="G86">
+        <v>4.99428592696275E-2</v>
+      </c>
+      <c r="H86">
+        <v>6.5068386110087298E-3</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>651</v>
+      </c>
+      <c r="B87" t="s">
+        <v>621</v>
+      </c>
+      <c r="C87">
+        <v>0.12438127476989699</v>
+      </c>
+      <c r="D87">
+        <v>4.3278419288159002E-2</v>
+      </c>
+      <c r="E87">
+        <v>0.62190637384948699</v>
+      </c>
+      <c r="F87">
+        <v>0.21639209644079499</v>
+      </c>
+      <c r="G87">
+        <v>0.12438127476989699</v>
+      </c>
+      <c r="H87">
+        <v>4.3278419288159002E-2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>290</v>
+      </c>
+      <c r="B88" t="s">
+        <v>631</v>
+      </c>
+      <c r="C88">
+        <v>0.96844081361221102</v>
+      </c>
+      <c r="D88">
+        <v>0.111730300400325</v>
+      </c>
+      <c r="E88">
+        <v>6.7790856952854703</v>
+      </c>
+      <c r="F88">
+        <v>0.78211210280227506</v>
+      </c>
+      <c r="G88">
+        <v>0.96844081361221102</v>
+      </c>
+      <c r="H88">
+        <v>0.111730300400325</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>290</v>
+      </c>
+      <c r="B89" t="s">
+        <v>622</v>
+      </c>
+      <c r="C89">
+        <v>0.132216516127214</v>
+      </c>
+      <c r="D89">
+        <v>5.5114076296368303E-2</v>
+      </c>
+      <c r="E89">
+        <v>0.925515612890498</v>
+      </c>
+      <c r="F89">
+        <v>0.38579853407457798</v>
+      </c>
+      <c r="G89">
+        <v>0.132216516127214</v>
+      </c>
+      <c r="H89">
+        <v>5.5114076296368303E-2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>290</v>
+      </c>
+      <c r="B90" t="s">
+        <v>620</v>
+      </c>
+      <c r="C90">
+        <v>0.20617736064313999</v>
+      </c>
+      <c r="D90">
+        <v>5.2648552284573699E-2</v>
+      </c>
+      <c r="E90">
+        <v>1.4432415245019801</v>
+      </c>
+      <c r="F90">
+        <v>0.36853986599201599</v>
+      </c>
+      <c r="G90">
+        <v>0.20617736064313999</v>
+      </c>
+      <c r="H90">
+        <v>5.2648552284573699E-2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>290</v>
+      </c>
+      <c r="B91" t="s">
+        <v>621</v>
+      </c>
+      <c r="C91">
+        <v>0.18734882973845299</v>
+      </c>
+      <c r="D91">
+        <v>2.2286044427989801E-2</v>
+      </c>
+      <c r="E91">
+        <v>1.3114418081691701</v>
+      </c>
+      <c r="F91">
+        <v>0.15600231099592901</v>
+      </c>
+      <c r="G91">
+        <v>0.18734882973845299</v>
+      </c>
+      <c r="H91">
+        <v>2.2286044427989801E-2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>308</v>
+      </c>
+      <c r="B92" t="s">
+        <v>631</v>
+      </c>
+      <c r="C92">
+        <v>48.534014257275999</v>
+      </c>
+      <c r="D92">
+        <v>8.7716278954898197</v>
+      </c>
+      <c r="E92">
+        <v>145.602042771828</v>
+      </c>
+      <c r="F92">
+        <v>26.3148836864694</v>
+      </c>
+      <c r="G92">
+        <v>48.534014257275999</v>
+      </c>
+      <c r="H92">
+        <v>8.7716278954898197</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>308</v>
+      </c>
+      <c r="B93" t="s">
+        <v>622</v>
+      </c>
+      <c r="C93">
+        <v>0.88574349844183198</v>
+      </c>
+      <c r="D93">
+        <v>0.11233300390425401</v>
+      </c>
+      <c r="E93">
+        <v>2.6572304953254902</v>
+      </c>
+      <c r="F93">
+        <v>0.33699901171276297</v>
+      </c>
+      <c r="G93">
+        <v>0.88574349844183198</v>
+      </c>
+      <c r="H93">
+        <v>0.11233300390425401</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>308</v>
+      </c>
+      <c r="B94" t="s">
+        <v>620</v>
+      </c>
+      <c r="C94">
+        <v>3.7178303669590398</v>
+      </c>
+      <c r="D94">
+        <v>0.92201365306087701</v>
+      </c>
+      <c r="E94">
+        <v>11.153491100877099</v>
+      </c>
+      <c r="F94">
+        <v>2.76604095918263</v>
+      </c>
+      <c r="G94">
+        <v>3.7178303669590398</v>
+      </c>
+      <c r="H94">
+        <v>0.92201365306087701</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>308</v>
+      </c>
+      <c r="B95" t="s">
+        <v>621</v>
+      </c>
+      <c r="C95">
+        <v>2.2445677481585702</v>
+      </c>
+      <c r="D95">
+        <v>0.15950140028808499</v>
+      </c>
+      <c r="E95">
+        <v>6.7337032444757101</v>
+      </c>
+      <c r="F95">
+        <v>0.47850420086425599</v>
+      </c>
+      <c r="G95">
+        <v>2.2445677481585702</v>
+      </c>
+      <c r="H95">
+        <v>0.15950140028808499</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>652</v>
+      </c>
+      <c r="B96" t="s">
+        <v>631</v>
+      </c>
+      <c r="C96">
+        <v>0.23297642131170099</v>
+      </c>
+      <c r="D96">
+        <v>1.7757235148504E-2</v>
+      </c>
+      <c r="E96">
+        <v>1.3978585278702</v>
+      </c>
+      <c r="F96">
+        <v>0.106543410891024</v>
+      </c>
+      <c r="G96">
+        <v>0.23297642131170099</v>
+      </c>
+      <c r="H96">
+        <v>1.7757235148504E-2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>652</v>
+      </c>
+      <c r="B97" t="s">
+        <v>622</v>
+      </c>
+      <c r="C97">
+        <v>5.4464563069325102E-2</v>
+      </c>
+      <c r="D97">
+        <v>1.6772918157421001E-2</v>
+      </c>
+      <c r="E97">
+        <v>0.32678737841595101</v>
+      </c>
+      <c r="F97">
+        <v>0.100637508944526</v>
+      </c>
+      <c r="G97">
+        <v>5.4464563069325102E-2</v>
+      </c>
+      <c r="H97">
+        <v>1.6772918157421001E-2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>652</v>
+      </c>
+      <c r="B98" t="s">
+        <v>620</v>
+      </c>
+      <c r="C98">
+        <v>0.15134464422376301</v>
+      </c>
+      <c r="D98">
+        <v>3.55041173738306E-2</v>
+      </c>
+      <c r="E98">
+        <v>0.908067865342578</v>
+      </c>
+      <c r="F98">
+        <v>0.213024704242983</v>
+      </c>
+      <c r="G98">
+        <v>0.15134464422376301</v>
+      </c>
+      <c r="H98">
+        <v>3.55041173738306E-2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>652</v>
+      </c>
+      <c r="B99" t="s">
+        <v>621</v>
+      </c>
+      <c r="C99">
+        <v>3.0431700937942501</v>
+      </c>
+      <c r="D99">
+        <v>0.36955309373200601</v>
+      </c>
+      <c r="E99">
+        <v>18.2590205627655</v>
+      </c>
+      <c r="F99">
+        <v>2.2173185623920402</v>
+      </c>
+      <c r="G99">
+        <v>3.0431700937942501</v>
+      </c>
+      <c r="H99">
+        <v>0.36955309373200601</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>653</v>
+      </c>
+      <c r="B100" t="s">
+        <v>631</v>
+      </c>
+      <c r="C100">
+        <v>2.4121693893054599</v>
+      </c>
+      <c r="D100">
+        <v>0.73352507212773499</v>
+      </c>
+      <c r="E100">
+        <v>21.709524503749201</v>
+      </c>
+      <c r="F100">
+        <v>6.6017256491496097</v>
+      </c>
+      <c r="G100">
+        <v>2.4121693893054599</v>
+      </c>
+      <c r="H100">
+        <v>0.73352507212773499</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>653</v>
+      </c>
+      <c r="B101" t="s">
+        <v>622</v>
+      </c>
+      <c r="C101">
+        <v>1.5443846598602999</v>
+      </c>
+      <c r="D101">
+        <v>0.57303249151865698</v>
+      </c>
+      <c r="E101">
+        <v>13.8994619387427</v>
+      </c>
+      <c r="F101">
+        <v>5.1572924236679096</v>
+      </c>
+      <c r="G101">
+        <v>1.5443846598602999</v>
+      </c>
+      <c r="H101">
+        <v>0.57303249151865698</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>312</v>
+      </c>
+      <c r="B102" t="s">
+        <v>631</v>
+      </c>
+      <c r="C102">
+        <v>1.5389935163453E-2</v>
+      </c>
+      <c r="D102">
+        <v>1.18025836217304E-3</v>
+      </c>
+      <c r="E102">
+        <v>7.6949675817265306E-2</v>
+      </c>
+      <c r="F102">
+        <v>5.9012918108652399E-3</v>
+      </c>
+      <c r="G102" t="s">
+        <v>322</v>
+      </c>
+      <c r="H102" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>654</v>
+      </c>
+      <c r="B103" t="s">
+        <v>631</v>
+      </c>
+      <c r="C103">
+        <v>16.333450355102599</v>
+      </c>
+      <c r="D103">
+        <v>2.0413888222410401</v>
+      </c>
+      <c r="E103">
+        <v>49.000351065308003</v>
+      </c>
+      <c r="F103">
+        <v>6.1241664667231301</v>
+      </c>
+      <c r="G103">
+        <v>16.333450355102599</v>
+      </c>
+      <c r="H103">
+        <v>2.0413888222410401</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>654</v>
+      </c>
+      <c r="B104" t="s">
+        <v>622</v>
+      </c>
+      <c r="C104">
+        <v>9.1909688589005096</v>
+      </c>
+      <c r="D104">
+        <v>0.60998113698647305</v>
+      </c>
+      <c r="E104">
+        <v>27.572906576701499</v>
+      </c>
+      <c r="F104">
+        <v>1.8299434109594099</v>
+      </c>
+      <c r="G104">
+        <v>9.1909688589005096</v>
+      </c>
+      <c r="H104">
+        <v>0.60998113698647305</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>654</v>
+      </c>
+      <c r="B105" t="s">
+        <v>620</v>
+      </c>
+      <c r="C105">
+        <v>2.7387159850923402</v>
+      </c>
+      <c r="D105">
+        <v>0.347696208365743</v>
+      </c>
+      <c r="E105">
+        <v>8.2161479552770302</v>
+      </c>
+      <c r="F105">
+        <v>1.04308862509723</v>
+      </c>
+      <c r="G105">
+        <v>2.7387159850923402</v>
+      </c>
+      <c r="H105">
+        <v>0.347696208365743</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>654</v>
+      </c>
+      <c r="B106" t="s">
+        <v>621</v>
+      </c>
+      <c r="C106">
+        <v>7.1593257665805803</v>
+      </c>
+      <c r="D106">
+        <v>1.0276099412826201</v>
+      </c>
+      <c r="E106">
+        <v>21.477977299741699</v>
+      </c>
+      <c r="F106">
+        <v>3.08282982384788</v>
+      </c>
+      <c r="G106">
+        <v>7.1593257665805803</v>
+      </c>
+      <c r="H106">
+        <v>1.0276099412826201</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>655</v>
+      </c>
+      <c r="B107" t="s">
+        <v>631</v>
+      </c>
+      <c r="C107">
+        <v>7.8969719236072402</v>
+      </c>
+      <c r="D107">
+        <v>0.99335500295351498</v>
+      </c>
+      <c r="E107">
+        <v>39.484859618036197</v>
+      </c>
+      <c r="F107">
+        <v>4.9667750147675704</v>
+      </c>
+      <c r="G107">
+        <v>7.8969719236072402</v>
+      </c>
+      <c r="H107">
+        <v>0.99335500295351498</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>655</v>
+      </c>
+      <c r="B108" t="s">
+        <v>622</v>
+      </c>
+      <c r="C108">
+        <v>3.4746774423364402</v>
+      </c>
+      <c r="D108">
+        <v>0.42958486288697101</v>
+      </c>
+      <c r="E108">
+        <v>17.3733872116822</v>
+      </c>
+      <c r="F108">
+        <v>2.1479243144348499</v>
+      </c>
+      <c r="G108">
+        <v>3.4746774423364402</v>
+      </c>
+      <c r="H108">
+        <v>0.42958486288697101</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>655</v>
+      </c>
+      <c r="B109" t="s">
+        <v>620</v>
+      </c>
+      <c r="C109">
+        <v>1.33047332074845</v>
+      </c>
+      <c r="D109">
+        <v>0.150194376242862</v>
+      </c>
+      <c r="E109">
+        <v>6.6523666037422799</v>
+      </c>
+      <c r="F109">
+        <v>0.75097188121431202</v>
+      </c>
+      <c r="G109">
+        <v>1.33047332074845</v>
+      </c>
+      <c r="H109">
+        <v>0.150194376242862</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
+        <v>655</v>
+      </c>
+      <c r="B110" t="s">
+        <v>621</v>
+      </c>
+      <c r="C110">
+        <v>1.4669151769320099</v>
+      </c>
+      <c r="D110">
+        <v>0.26311450007942899</v>
+      </c>
+      <c r="E110">
+        <v>7.3345758846600599</v>
+      </c>
+      <c r="F110">
+        <v>1.3155725003971399</v>
+      </c>
+      <c r="G110">
+        <v>1.4669151769320099</v>
+      </c>
+      <c r="H110">
+        <v>0.26311450007942899</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
+        <v>656</v>
+      </c>
+      <c r="B111" t="s">
+        <v>631</v>
+      </c>
+      <c r="C111">
+        <v>3.1088518562957401</v>
+      </c>
+      <c r="D111">
+        <v>0.27578767371172602</v>
+      </c>
+      <c r="E111">
+        <v>15.5442592814787</v>
+      </c>
+      <c r="F111">
+        <v>1.3789383685586301</v>
+      </c>
+      <c r="G111">
+        <v>3.1088518562957401</v>
+      </c>
+      <c r="H111">
+        <v>0.27578767371172602</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
+        <v>656</v>
+      </c>
+      <c r="B112" t="s">
+        <v>620</v>
+      </c>
+      <c r="C112">
+        <v>2.8076019634173099</v>
+      </c>
+      <c r="D112">
+        <v>5.3928324294668102E-2</v>
+      </c>
+      <c r="E112">
+        <v>14.0380098170865</v>
+      </c>
+      <c r="F112">
+        <v>0.26964162147333998</v>
+      </c>
+      <c r="G112">
+        <v>2.8076019634173099</v>
+      </c>
+      <c r="H112">
+        <v>5.3928324294668102E-2</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
+        <v>656</v>
+      </c>
+      <c r="B113" t="s">
+        <v>621</v>
+      </c>
+      <c r="C113">
+        <v>5.2029343250868099</v>
+      </c>
+      <c r="D113">
+        <v>0.192486613759319</v>
+      </c>
+      <c r="E113">
+        <v>26.014671625434001</v>
+      </c>
+      <c r="F113">
+        <v>0.96243306879659996</v>
+      </c>
+      <c r="G113">
+        <v>5.2029343250868099</v>
+      </c>
+      <c r="H113">
+        <v>0.192486613759319</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>392</v>
+      </c>
+      <c r="B114" t="s">
+        <v>631</v>
+      </c>
+      <c r="C114">
+        <v>0.46761622350071802</v>
+      </c>
+      <c r="D114">
+        <v>5.1083785095388398E-2</v>
+      </c>
+      <c r="E114">
+        <v>1.8704648940028701</v>
+      </c>
+      <c r="F114">
+        <v>0.20433514038155301</v>
+      </c>
+      <c r="G114">
+        <v>1.4028486705021499</v>
+      </c>
+      <c r="H114">
+        <v>0.15325135528616499</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
+        <v>392</v>
+      </c>
+      <c r="B115" t="s">
+        <v>622</v>
+      </c>
+      <c r="C115">
+        <v>1.21313566849817</v>
+      </c>
+      <c r="D115">
+        <v>0.109460703991396</v>
+      </c>
+      <c r="E115">
+        <v>4.8525426739927102</v>
+      </c>
+      <c r="F115">
+        <v>0.437842815965585</v>
+      </c>
+      <c r="G115">
+        <v>3.63940700549453</v>
+      </c>
+      <c r="H115">
+        <v>0.32838211197418798</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>392</v>
+      </c>
+      <c r="B116" t="s">
+        <v>620</v>
+      </c>
+      <c r="C116">
+        <v>0.912217693407818</v>
+      </c>
+      <c r="D116">
+        <v>0.275468197800535</v>
+      </c>
+      <c r="E116">
+        <v>3.6488707736312702</v>
+      </c>
+      <c r="F116">
+        <v>1.10187279120214</v>
+      </c>
+      <c r="G116">
+        <v>2.7366530802234501</v>
+      </c>
+      <c r="H116">
+        <v>0.82640459340160699</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
+        <v>392</v>
+      </c>
+      <c r="B117" t="s">
+        <v>621</v>
+      </c>
+      <c r="C117">
+        <v>1.39756449340334</v>
+      </c>
+      <c r="D117">
+        <v>7.5459385695331199E-2</v>
+      </c>
+      <c r="E117">
+        <v>5.59025797361336</v>
+      </c>
+      <c r="F117">
+        <v>0.30183754278132402</v>
+      </c>
+      <c r="G117">
+        <v>4.1926934802100204</v>
+      </c>
+      <c r="H117">
+        <v>0.22637815708599299</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
+        <v>484</v>
+      </c>
+      <c r="B118" t="s">
+        <v>621</v>
+      </c>
+      <c r="C118">
+        <v>9.2187343275653102E-2</v>
+      </c>
+      <c r="D118">
+        <v>9.4322730317052492E-3</v>
+      </c>
+      <c r="E118">
+        <v>0.460936716378265</v>
+      </c>
+      <c r="F118">
+        <v>4.7161365158526203E-2</v>
+      </c>
+      <c r="G118">
+        <v>0.36874937310261202</v>
+      </c>
+      <c r="H118">
+        <v>3.7729092126820997E-2</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
+        <v>657</v>
+      </c>
+      <c r="B119" t="s">
+        <v>631</v>
+      </c>
+      <c r="C119">
+        <v>0.62252388613077103</v>
+      </c>
+      <c r="D119">
+        <v>0.14103241545181699</v>
+      </c>
+      <c r="E119">
+        <v>5.6027149751769398</v>
+      </c>
+      <c r="F119">
+        <v>1.2692917390663501</v>
+      </c>
+      <c r="G119">
+        <v>0.62252388613077103</v>
+      </c>
+      <c r="H119">
+        <v>0.14103241545181699</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
+        <v>657</v>
+      </c>
+      <c r="B120" t="s">
+        <v>621</v>
+      </c>
+      <c r="C120">
+        <v>0.55586617481915401</v>
+      </c>
+      <c r="D120">
+        <v>3.5252953359035798E-2</v>
+      </c>
+      <c r="E120">
+        <v>5.0027955733723903</v>
+      </c>
+      <c r="F120">
+        <v>0.31727658023132299</v>
+      </c>
+      <c r="G120">
+        <v>0.55586617481915401</v>
+      </c>
+      <c r="H120">
+        <v>3.5252953359035798E-2</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C39A3B0E-7A89-3F4E-AFD3-E9F41AB675B1}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" t="s">
+        <v>616</v>
+      </c>
+      <c r="C1" t="s">
+        <v>624</v>
+      </c>
+      <c r="D1" t="s">
+        <v>625</v>
+      </c>
+      <c r="E1" t="s">
+        <v>626</v>
+      </c>
+      <c r="F1" t="s">
+        <v>627</v>
+      </c>
+      <c r="G1" t="s">
+        <v>628</v>
+      </c>
+      <c r="H1" t="s">
+        <v>629</v>
+      </c>
+      <c r="I1" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>633</v>
+      </c>
+      <c r="B2" t="s">
+        <v>631</v>
+      </c>
+      <c r="C2">
+        <v>6.6238726389443699E-3</v>
+      </c>
+      <c r="D2" s="6">
+        <v>5.06869014189796E-4</v>
+      </c>
+      <c r="E2">
+        <v>3.97432358336662E-2</v>
+      </c>
+      <c r="F2">
+        <v>3.0412140851387701E-3</v>
+      </c>
+      <c r="G2">
+        <v>3.31193631947218E-2</v>
+      </c>
+      <c r="H2">
+        <v>2.5343450709489801E-3</v>
+      </c>
+      <c r="I2">
+        <v>3.9649467742451996E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>633</v>
+      </c>
+      <c r="B3" t="s">
+        <v>621</v>
+      </c>
+      <c r="C3">
+        <v>1.48435260897338E-2</v>
+      </c>
+      <c r="D3">
+        <v>5.2056241192211597E-3</v>
+      </c>
+      <c r="E3">
+        <v>8.9061156538403005E-2</v>
+      </c>
+      <c r="F3">
+        <v>3.1233744715326899E-2</v>
+      </c>
+      <c r="G3">
+        <v>7.4217630448669206E-2</v>
+      </c>
+      <c r="H3">
+        <v>2.6028120596105798E-2</v>
+      </c>
+      <c r="I3">
+        <v>3.9649467742451996E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>659</v>
+      </c>
+      <c r="B4" t="s">
+        <v>631</v>
+      </c>
+      <c r="C4">
+        <v>0.679336080507006</v>
+      </c>
+      <c r="D4">
+        <v>0.39318604625114401</v>
+      </c>
+      <c r="E4">
+        <v>4.0760164830420296</v>
+      </c>
+      <c r="F4">
+        <v>2.3591162775068599</v>
+      </c>
+      <c r="G4" t="s">
+        <v>322</v>
+      </c>
+      <c r="H4" t="s">
+        <v>322</v>
+      </c>
+      <c r="I4">
+        <v>0.138498009009657</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>659</v>
+      </c>
+      <c r="B5" t="s">
+        <v>621</v>
+      </c>
+      <c r="C5">
+        <v>1.0810509986555601</v>
+      </c>
+      <c r="D5">
+        <v>0.25791222143770998</v>
+      </c>
+      <c r="E5">
+        <v>6.4863059919333903</v>
+      </c>
+      <c r="F5">
+        <v>1.5474733286262601</v>
+      </c>
+      <c r="G5" t="s">
+        <v>322</v>
+      </c>
+      <c r="H5" t="s">
+        <v>322</v>
+      </c>
+      <c r="I5">
+        <v>0.138498009009657</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>390</v>
+      </c>
+      <c r="B6" t="s">
+        <v>631</v>
+      </c>
+      <c r="C6">
+        <v>8.1385237556089396E-2</v>
+      </c>
+      <c r="D6">
+        <v>1.33664524567721E-2</v>
+      </c>
+      <c r="E6">
+        <v>0.40692618778044698</v>
+      </c>
+      <c r="F6">
+        <v>6.6832262283860897E-2</v>
+      </c>
+      <c r="G6">
+        <v>0.40692618778044698</v>
+      </c>
+      <c r="H6">
+        <v>6.6832262283860897E-2</v>
+      </c>
+      <c r="I6">
+        <v>6.4103845329483794E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>390</v>
+      </c>
+      <c r="B7" t="s">
+        <v>621</v>
+      </c>
+      <c r="C7">
+        <v>0.17364707087174999</v>
+      </c>
+      <c r="D7">
+        <v>6.8246044806423004E-2</v>
+      </c>
+      <c r="E7">
+        <v>0.86823535435875099</v>
+      </c>
+      <c r="F7">
+        <v>0.341230224032115</v>
+      </c>
+      <c r="G7">
+        <v>0.86823535435875099</v>
+      </c>
+      <c r="H7">
+        <v>0.341230224032115</v>
+      </c>
+      <c r="I7">
+        <v>6.4103845329483794E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>400</v>
+      </c>
+      <c r="B8" t="s">
+        <v>631</v>
+      </c>
+      <c r="C8">
+        <v>1.5021972260061999E-2</v>
+      </c>
+      <c r="D8">
+        <v>2.2194705947714598E-3</v>
+      </c>
+      <c r="E8">
+        <v>0.150219722600621</v>
+      </c>
+      <c r="F8">
+        <v>2.21947059477146E-2</v>
+      </c>
+      <c r="G8">
+        <v>7.5109861300310499E-2</v>
+      </c>
+      <c r="H8">
+        <v>1.10973529738573E-2</v>
+      </c>
+      <c r="I8">
+        <v>1.4156475538651401E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>400</v>
+      </c>
+      <c r="B9" t="s">
+        <v>621</v>
+      </c>
+      <c r="C9">
+        <v>9.4578862515319995E-2</v>
+      </c>
+      <c r="D9">
+        <v>7.8578834760376099E-3</v>
+      </c>
+      <c r="E9">
+        <v>0.94578862515319995</v>
+      </c>
+      <c r="F9">
+        <v>7.8578834760376096E-2</v>
+      </c>
+      <c r="G9">
+        <v>0.47289431257659997</v>
+      </c>
+      <c r="H9">
+        <v>3.9289417380187999E-2</v>
+      </c>
+      <c r="I9">
+        <v>1.4156475538651401E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>379</v>
+      </c>
+      <c r="B10" t="s">
+        <v>631</v>
+      </c>
+      <c r="C10">
+        <v>5.0084141077925998E-2</v>
+      </c>
+      <c r="D10">
+        <v>2.4283669306022201E-2</v>
+      </c>
+      <c r="E10">
+        <v>0.70117797509096402</v>
+      </c>
+      <c r="F10">
+        <v>0.33997137028431101</v>
+      </c>
+      <c r="G10">
+        <v>0.100168282155852</v>
+      </c>
+      <c r="H10">
+        <v>4.8567338612044403E-2</v>
+      </c>
+      <c r="I10">
+        <v>7.42284694967431E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>379</v>
+      </c>
+      <c r="B11" t="s">
+        <v>621</v>
+      </c>
+      <c r="C11">
+        <v>6.9979049221835704E-2</v>
+      </c>
+      <c r="D11">
+        <v>4.3525205532674402E-2</v>
+      </c>
+      <c r="E11">
+        <v>0.97970668910570002</v>
+      </c>
+      <c r="F11">
+        <v>0.60935287745744204</v>
+      </c>
+      <c r="G11">
+        <v>0.13995809844367099</v>
+      </c>
+      <c r="H11">
+        <v>8.7050411065348901E-2</v>
+      </c>
+      <c r="I11">
+        <v>7.42284694967431E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>323</v>
+      </c>
+      <c r="B12" t="s">
+        <v>631</v>
+      </c>
+      <c r="C12">
+        <v>1.1912017033481801</v>
+      </c>
+      <c r="D12">
+        <v>0.331367441602824</v>
+      </c>
+      <c r="E12">
+        <v>8.3384119234373095</v>
+      </c>
+      <c r="F12">
+        <v>2.3195720912197699</v>
+      </c>
+      <c r="G12" t="s">
+        <v>322</v>
+      </c>
+      <c r="H12" t="s">
+        <v>322</v>
+      </c>
+      <c r="I12">
+        <v>7.6504208874445506E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>323</v>
+      </c>
+      <c r="B13" t="s">
+        <v>621</v>
+      </c>
+      <c r="C13">
+        <v>0.99358230038542295</v>
+      </c>
+      <c r="D13">
+        <v>0.29925426315728698</v>
+      </c>
+      <c r="E13">
+        <v>6.9550761026979604</v>
+      </c>
+      <c r="F13">
+        <v>2.0947798421010102</v>
+      </c>
+      <c r="G13" t="s">
+        <v>322</v>
+      </c>
+      <c r="H13" t="s">
+        <v>322</v>
+      </c>
+      <c r="I13">
+        <v>7.6504208874445506E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>394</v>
+      </c>
+      <c r="B14" t="s">
+        <v>631</v>
+      </c>
+      <c r="C14">
+        <v>0.93927227053055395</v>
+      </c>
+      <c r="D14">
+        <v>0.118633796418886</v>
+      </c>
+      <c r="E14">
+        <v>4.6963613526527697</v>
+      </c>
+      <c r="F14">
+        <v>0.59316898209443203</v>
+      </c>
+      <c r="G14">
+        <v>4.6963613526527697</v>
+      </c>
+      <c r="H14">
+        <v>0.59316898209443203</v>
+      </c>
+      <c r="I14">
+        <v>0.42813712446103702</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>394</v>
+      </c>
+      <c r="B15" t="s">
+        <v>621</v>
+      </c>
+      <c r="C15">
+        <v>2.3070705103004401</v>
+      </c>
+      <c r="D15">
+        <v>0.466800411074758</v>
+      </c>
+      <c r="E15">
+        <v>11.5353525515022</v>
+      </c>
+      <c r="F15">
+        <v>2.3340020553737899</v>
+      </c>
+      <c r="G15">
+        <v>11.5353525515022</v>
+      </c>
+      <c r="H15">
+        <v>2.3340020553737899</v>
+      </c>
+      <c r="I15">
+        <v>0.42813712446103702</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>644</v>
+      </c>
+      <c r="B16" t="s">
+        <v>631</v>
+      </c>
+      <c r="C16">
+        <v>3.9937168025485601</v>
+      </c>
+      <c r="D16">
+        <v>0.17366257653237999</v>
+      </c>
+      <c r="E16">
+        <v>23.9623008152913</v>
+      </c>
+      <c r="F16">
+        <v>1.04197545919428</v>
+      </c>
+      <c r="G16">
+        <v>3.9937168025485601</v>
+      </c>
+      <c r="H16">
+        <v>0.17366257653237999</v>
+      </c>
+      <c r="I16">
+        <v>0.12958842183483199</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>644</v>
+      </c>
+      <c r="B17" t="s">
+        <v>621</v>
+      </c>
+      <c r="C17">
+        <v>1.7214478102250399</v>
+      </c>
+      <c r="D17">
+        <v>0.16194909704569699</v>
+      </c>
+      <c r="E17">
+        <v>10.328686861350199</v>
+      </c>
+      <c r="F17">
+        <v>0.97169458227418604</v>
+      </c>
+      <c r="G17">
+        <v>1.7214478102250399</v>
+      </c>
+      <c r="H17">
+        <v>0.16194909704569699</v>
+      </c>
+      <c r="I17">
+        <v>0.12958842183483199</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>367</v>
+      </c>
+      <c r="B18" t="s">
+        <v>631</v>
+      </c>
+      <c r="C18">
+        <v>0.26657604259484102</v>
+      </c>
+      <c r="D18">
+        <v>5.8486715097868298E-2</v>
+      </c>
+      <c r="E18">
+        <v>2.9323364685432498</v>
+      </c>
+      <c r="F18">
+        <v>0.64335386607655098</v>
+      </c>
+      <c r="G18">
+        <v>0.26657604259484102</v>
+      </c>
+      <c r="H18">
+        <v>5.8486715097868298E-2</v>
+      </c>
+      <c r="I18">
+        <v>2.2282808012933499E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>367</v>
+      </c>
+      <c r="B19" t="s">
+        <v>621</v>
+      </c>
+      <c r="C19">
+        <v>0.21798032239996601</v>
+      </c>
+      <c r="D19">
+        <v>1.8697227558770999E-2</v>
+      </c>
+      <c r="E19">
+        <v>2.3977835463996202</v>
+      </c>
+      <c r="F19">
+        <v>0.205669503146482</v>
+      </c>
+      <c r="G19">
+        <v>0.21798032239996601</v>
+      </c>
+      <c r="H19">
+        <v>1.8697227558770999E-2</v>
+      </c>
+      <c r="I19">
+        <v>2.2282808012933499E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>660</v>
+      </c>
+      <c r="B20" t="s">
+        <v>621</v>
+      </c>
+      <c r="C20">
+        <v>3.5660205759188102E-2</v>
+      </c>
+      <c r="D20">
+        <v>1.36474695326715E-2</v>
+      </c>
+      <c r="E20">
+        <v>0.24962144031431599</v>
+      </c>
+      <c r="F20">
+        <v>9.5532286728700705E-2</v>
+      </c>
+      <c r="G20" t="s">
+        <v>322</v>
+      </c>
+      <c r="H20" t="s">
+        <v>322</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>653</v>
+      </c>
+      <c r="B21" t="s">
+        <v>631</v>
+      </c>
+      <c r="C21">
+        <v>2.3907482750919198</v>
+      </c>
+      <c r="D21">
+        <v>0.26274509254762402</v>
+      </c>
+      <c r="E21">
+        <v>21.516734475827299</v>
+      </c>
+      <c r="F21">
+        <v>2.3647058329286099</v>
+      </c>
+      <c r="G21">
+        <v>2.3907482750919198</v>
+      </c>
+      <c r="H21">
+        <v>0.26274509254762402</v>
+      </c>
+      <c r="I21">
+        <v>0.39827474663971002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>653</v>
+      </c>
+      <c r="B22" t="s">
+        <v>621</v>
+      </c>
+      <c r="C22">
+        <v>1.0586054880525799</v>
+      </c>
+      <c r="D22">
+        <v>1.8350805416927001E-2</v>
+      </c>
+      <c r="E22">
+        <v>9.5274493924732209</v>
+      </c>
+      <c r="F22">
+        <v>0.165157248752343</v>
+      </c>
+      <c r="G22">
+        <v>1.0586054880525799</v>
+      </c>
+      <c r="H22">
+        <v>1.8350805416927001E-2</v>
+      </c>
+      <c r="I22">
+        <v>0.39827474663971002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>661</v>
+      </c>
+      <c r="B23" t="s">
+        <v>631</v>
+      </c>
+      <c r="C23">
+        <v>1.0783601029269899E-2</v>
+      </c>
+      <c r="D23">
+        <v>3.16930148909891E-3</v>
+      </c>
+      <c r="E23">
+        <v>0.15097041440977799</v>
+      </c>
+      <c r="F23">
+        <v>4.4370220847384803E-2</v>
+      </c>
+      <c r="G23">
+        <v>6.4701606175619403E-2</v>
+      </c>
+      <c r="H23">
+        <v>1.9015808934593401E-2</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>661</v>
+      </c>
+      <c r="B24" t="s">
+        <v>621</v>
+      </c>
+      <c r="C24">
+        <v>1.02125782540223E-2</v>
+      </c>
+      <c r="D24">
+        <v>2.3615268504354301E-3</v>
+      </c>
+      <c r="E24">
+        <v>0.14297609555631199</v>
+      </c>
+      <c r="F24">
+        <v>3.3061375906096098E-2</v>
+      </c>
+      <c r="G24">
+        <v>6.1275469524133902E-2</v>
+      </c>
+      <c r="H24">
+        <v>1.41691611026126E-2</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>662</v>
+      </c>
+      <c r="B25" t="s">
+        <v>631</v>
+      </c>
+      <c r="C25">
+        <v>4.1582827991513503E-3</v>
+      </c>
+      <c r="D25" s="6">
+        <v>7.4063232065494299E-4</v>
+      </c>
+      <c r="E25">
+        <v>6.2374241987270297E-2</v>
+      </c>
+      <c r="F25">
+        <v>1.1109484809824099E-2</v>
+      </c>
+      <c r="G25">
+        <v>4.1582827991513503E-3</v>
+      </c>
+      <c r="H25" s="6">
+        <v>7.4063232065494299E-4</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>662</v>
+      </c>
+      <c r="B26" t="s">
+        <v>621</v>
+      </c>
+      <c r="C26">
+        <v>1.16827945298674E-2</v>
+      </c>
+      <c r="D26">
+        <v>1.1492789973712199E-2</v>
+      </c>
+      <c r="E26">
+        <v>0.175241917948011</v>
+      </c>
+      <c r="F26">
+        <v>0.17239184960568299</v>
+      </c>
+      <c r="G26">
+        <v>1.16827945298674E-2</v>
+      </c>
+      <c r="H26">
+        <v>1.1492789973712199E-2</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>663</v>
+      </c>
+      <c r="B27" t="s">
+        <v>631</v>
+      </c>
+      <c r="C27">
+        <v>3.4053957467854702E-2</v>
+      </c>
+      <c r="D27">
+        <v>3.3845790821469601E-2</v>
+      </c>
+      <c r="E27">
+        <v>0.34053957467854701</v>
+      </c>
+      <c r="F27">
+        <v>0.33845790821469601</v>
+      </c>
+      <c r="G27">
+        <v>6.8107914935709404E-2</v>
+      </c>
+      <c r="H27">
+        <v>6.7691581642939203E-2</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>663</v>
+      </c>
+      <c r="B28" t="s">
+        <v>621</v>
+      </c>
+      <c r="C28">
+        <v>9.4524247414354501E-2</v>
+      </c>
+      <c r="D28">
+        <v>6.1072274931444001E-2</v>
+      </c>
+      <c r="E28">
+        <v>0.94524247414354501</v>
+      </c>
+      <c r="F28">
+        <v>0.61072274931444004</v>
+      </c>
+      <c r="G28">
+        <v>0.189048494828709</v>
+      </c>
+      <c r="H28">
+        <v>0.122144549862888</v>
+      </c>
+      <c r="I28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>557</v>
+      </c>
+      <c r="B29" t="s">
+        <v>631</v>
+      </c>
+      <c r="C29" s="6">
+        <v>1.7298358034433401E-4</v>
+      </c>
+      <c r="D29" s="6">
+        <v>1.3472015329543501E-4</v>
+      </c>
+      <c r="E29">
+        <v>1.9028193837876701E-3</v>
+      </c>
+      <c r="F29">
+        <v>1.48192168624979E-3</v>
+      </c>
+      <c r="G29" s="6">
+        <v>8.6491790172166997E-4</v>
+      </c>
+      <c r="H29" s="6">
+        <v>6.7360076647717698E-4</v>
+      </c>
+      <c r="I29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>557</v>
+      </c>
+      <c r="B30" t="s">
+        <v>621</v>
+      </c>
+      <c r="C30">
+        <v>1.4545965421603E-3</v>
+      </c>
+      <c r="D30">
+        <v>1.1012971352765701E-3</v>
+      </c>
+      <c r="E30">
+        <v>1.6000561963763298E-2</v>
+      </c>
+      <c r="F30">
+        <v>1.21142684880423E-2</v>
+      </c>
+      <c r="G30">
+        <v>7.2729827108015104E-3</v>
+      </c>
+      <c r="H30">
+        <v>5.5064856763828796E-3</v>
+      </c>
+      <c r="I30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>664</v>
+      </c>
+      <c r="B31" t="s">
+        <v>631</v>
+      </c>
+      <c r="C31">
+        <v>2.9894952965619898E-3</v>
+      </c>
+      <c r="D31" s="6">
+        <v>6.6506551440924001E-5</v>
+      </c>
+      <c r="E31">
+        <v>1.7936971779372E-2</v>
+      </c>
+      <c r="F31" s="6">
+        <v>3.9903930864555298E-4</v>
+      </c>
+      <c r="G31">
+        <v>2.9894952965619898E-3</v>
+      </c>
+      <c r="H31" s="6">
+        <v>6.6506551440924001E-5</v>
+      </c>
+      <c r="I31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>664</v>
+      </c>
+      <c r="B32" t="s">
+        <v>621</v>
+      </c>
+      <c r="C32">
+        <v>6.4607400584037701E-3</v>
+      </c>
+      <c r="D32" s="6">
+        <v>5.7328941756855595E-4</v>
+      </c>
+      <c r="E32">
+        <v>3.8764440350422598E-2</v>
+      </c>
+      <c r="F32">
+        <v>3.43973650541134E-3</v>
+      </c>
+      <c r="G32">
+        <v>6.4607400584037701E-3</v>
+      </c>
+      <c r="H32" s="6">
+        <v>5.7328941756855595E-4</v>
+      </c>
+      <c r="I32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>24</v>
+      </c>
+      <c r="B33" t="s">
+        <v>631</v>
+      </c>
+      <c r="C33">
+        <v>1.88756221696041E-2</v>
+      </c>
+      <c r="D33">
+        <v>8.4395113415418506E-3</v>
+      </c>
+      <c r="E33">
+        <v>0.20763184386564501</v>
+      </c>
+      <c r="F33">
+        <v>9.2834624756960304E-2</v>
+      </c>
+      <c r="G33">
+        <v>3.7751244339208199E-2</v>
+      </c>
+      <c r="H33">
+        <v>1.6879022683083701E-2</v>
+      </c>
+      <c r="I33">
+        <v>1.3677515133815499E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>24</v>
+      </c>
+      <c r="B34" t="s">
+        <v>621</v>
+      </c>
+      <c r="C34">
+        <v>1.8852454389459702E-2</v>
+      </c>
+      <c r="D34">
+        <v>5.2454087402661904E-3</v>
+      </c>
+      <c r="E34">
+        <v>0.20737699828405701</v>
+      </c>
+      <c r="F34">
+        <v>5.7699496142928103E-2</v>
+      </c>
+      <c r="G34">
+        <v>3.7704908778919501E-2</v>
+      </c>
+      <c r="H34">
+        <v>1.0490817480532299E-2</v>
+      </c>
+      <c r="I34">
+        <v>1.3677515133815499E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>665</v>
+      </c>
+      <c r="B35" t="s">
+        <v>631</v>
+      </c>
+      <c r="C35">
+        <v>7.2259663824697697E-3</v>
+      </c>
+      <c r="D35">
+        <v>4.2203845640389802E-3</v>
+      </c>
+      <c r="E35">
+        <v>4.3355798294818601E-2</v>
+      </c>
+      <c r="F35">
+        <v>2.53223073842339E-2</v>
+      </c>
+      <c r="G35">
+        <v>7.2259663824697697E-3</v>
+      </c>
+      <c r="H35">
+        <v>4.2203845640389802E-3</v>
+      </c>
+      <c r="I35">
+        <v>4.0652069064046103E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>665</v>
+      </c>
+      <c r="B36" t="s">
+        <v>621</v>
+      </c>
+      <c r="C36">
+        <v>1.1237141259429E-2</v>
+      </c>
+      <c r="D36">
+        <v>5.1510349830035896E-3</v>
+      </c>
+      <c r="E36">
+        <v>6.7422847556574295E-2</v>
+      </c>
+      <c r="F36">
+        <v>3.0906209898021501E-2</v>
+      </c>
+      <c r="G36">
+        <v>1.1237141259429E-2</v>
+      </c>
+      <c r="H36">
+        <v>5.1510349830035896E-3</v>
+      </c>
+      <c r="I36">
+        <v>4.0652069064046103E-3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>666</v>
+      </c>
+      <c r="B37" t="s">
+        <v>631</v>
+      </c>
+      <c r="C37">
+        <v>4.1751709181266604E-3</v>
+      </c>
+      <c r="D37" s="6">
+        <v>3.8970892686969298E-4</v>
+      </c>
+      <c r="E37">
+        <v>3.7576538263139898E-2</v>
+      </c>
+      <c r="F37">
+        <v>3.5073803418272402E-3</v>
+      </c>
+      <c r="G37">
+        <v>4.1751709181266604E-3</v>
+      </c>
+      <c r="H37" s="6">
+        <v>3.8970892686969298E-4</v>
+      </c>
+      <c r="I37">
+        <v>1.0744281736656E-3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>666</v>
+      </c>
+      <c r="B38" t="s">
+        <v>621</v>
+      </c>
+      <c r="C38">
+        <v>1.4188535819564E-2</v>
+      </c>
+      <c r="D38">
+        <v>2.0818463768113699E-3</v>
+      </c>
+      <c r="E38">
+        <v>0.12769682237607599</v>
+      </c>
+      <c r="F38">
+        <v>1.8736617391302401E-2</v>
+      </c>
+      <c r="G38">
+        <v>1.4188535819564E-2</v>
+      </c>
+      <c r="H38">
+        <v>2.0818463768113699E-3</v>
+      </c>
+      <c r="I38">
+        <v>1.0744281736656E-3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>667</v>
+      </c>
+      <c r="B39" t="s">
+        <v>631</v>
+      </c>
+      <c r="C39">
+        <v>1.4193095376173699E-2</v>
+      </c>
+      <c r="D39" s="6">
+        <v>9.2157069651173005E-4</v>
+      </c>
+      <c r="E39">
+        <v>0.11354476300939</v>
+      </c>
+      <c r="F39">
+        <v>7.3725655720938404E-3</v>
+      </c>
+      <c r="G39">
+        <v>1.4193095376173699E-2</v>
+      </c>
+      <c r="H39" s="6">
+        <v>9.2157069651173005E-4</v>
+      </c>
+      <c r="I39" s="6">
+        <v>4.1272426857691402E-4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>667</v>
+      </c>
+      <c r="B40" t="s">
+        <v>621</v>
+      </c>
+      <c r="C40">
+        <v>1.24705395880076E-2</v>
+      </c>
+      <c r="D40">
+        <v>1.4146658423729601E-3</v>
+      </c>
+      <c r="E40">
+        <v>9.9764316704060899E-2</v>
+      </c>
+      <c r="F40">
+        <v>1.13173267389837E-2</v>
+      </c>
+      <c r="G40">
+        <v>1.24705395880076E-2</v>
+      </c>
+      <c r="H40">
+        <v>1.4146658423729601E-3</v>
+      </c>
+      <c r="I40" s="6">
+        <v>4.1272426857691402E-4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>668</v>
+      </c>
+      <c r="B41" t="s">
+        <v>631</v>
+      </c>
+      <c r="C41">
+        <v>1.57526581996454E-2</v>
+      </c>
+      <c r="D41">
+        <v>1.8027443698331301E-3</v>
+      </c>
+      <c r="E41">
+        <v>0.29930050579326201</v>
+      </c>
+      <c r="F41">
+        <v>3.42521430268296E-2</v>
+      </c>
+      <c r="G41">
+        <v>0.110268607397517</v>
+      </c>
+      <c r="H41">
+        <v>1.26192105888319E-2</v>
+      </c>
+      <c r="I41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>668</v>
+      </c>
+      <c r="B42" t="s">
+        <v>621</v>
+      </c>
+      <c r="C42">
+        <v>2.3699346453558302E-2</v>
+      </c>
+      <c r="D42">
+        <v>1.2610790884456999E-2</v>
+      </c>
+      <c r="E42">
+        <v>0.45028758261760798</v>
+      </c>
+      <c r="F42">
+        <v>0.23960502680468301</v>
+      </c>
+      <c r="G42">
+        <v>0.16589542517490799</v>
+      </c>
+      <c r="H42">
+        <v>8.82755361911991E-2</v>
+      </c>
+      <c r="I42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>484</v>
+      </c>
+      <c r="B43" t="s">
+        <v>631</v>
+      </c>
+      <c r="C43">
+        <v>5.6797676429597701E-3</v>
+      </c>
+      <c r="D43">
+        <v>3.38687544336012E-3</v>
+      </c>
+      <c r="E43">
+        <v>2.83988382147989E-2</v>
+      </c>
+      <c r="F43">
+        <v>1.6934377216800599E-2</v>
+      </c>
+      <c r="G43">
+        <v>2.2719070571839101E-2</v>
+      </c>
+      <c r="H43">
+        <v>1.3547501773440499E-2</v>
+      </c>
+      <c r="I43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>484</v>
+      </c>
+      <c r="B44" t="s">
+        <v>621</v>
+      </c>
+      <c r="C44">
+        <v>2.34588773563798E-2</v>
+      </c>
+      <c r="D44">
+        <v>1.6245509522633001E-2</v>
+      </c>
+      <c r="E44">
+        <v>0.117294386781899</v>
+      </c>
+      <c r="F44">
+        <v>8.1227547613165293E-2</v>
+      </c>
+      <c r="G44">
+        <v>9.3835509425519506E-2</v>
+      </c>
+      <c r="H44">
+        <v>6.4982038090532199E-2</v>
+      </c>
+      <c r="I44">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>